<commit_message>
* Finished proofreading * Reworked diagrams * Added titlepage from FH
</commit_message>
<xml_diff>
--- a/latex/charts/2013_07_11_matrix.xlsx
+++ b/latex/charts/2013_07_11_matrix.xlsx
@@ -689,6 +689,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="19050"/>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -990,6 +993,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="19050"/>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1291,6 +1297,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="19050"/>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1593,7 +1602,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="19050">
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
@@ -1899,7 +1908,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="19050">
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
@@ -2205,7 +2214,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="19050">
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
@@ -2511,7 +2520,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="19050">
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
@@ -2810,11 +2819,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75435968"/>
-        <c:axId val="75436544"/>
+        <c:axId val="95621056"/>
+        <c:axId val="95621632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75435968"/>
+        <c:axId val="95621056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4000"/>
@@ -2844,12 +2853,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75436544"/>
+        <c:crossAx val="95621632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75436544"/>
+        <c:axId val="95621632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -2880,7 +2889,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75435968"/>
+        <c:crossAx val="95621056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2925,10 +2934,10 @@
       <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>8176</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>79424</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3239,8 +3248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M31" sqref="M30:N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
* Applied doblers feedback to sort chapter * rechecked all function names and corresponding chart series
</commit_message>
<xml_diff>
--- a/latex/charts/2013_07_11_matrix.xlsx
+++ b/latex/charts/2013_07_11_matrix.xlsx
@@ -2819,11 +2819,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95621056"/>
-        <c:axId val="95621632"/>
+        <c:axId val="89853888"/>
+        <c:axId val="89854464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95621056"/>
+        <c:axId val="89853888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4000"/>
@@ -2837,10 +2837,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Edge length</a:t>
                 </a:r>
               </a:p>
@@ -2853,12 +2853,22 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95621632"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="89854464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95621632"/>
+        <c:axId val="89854464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -2869,14 +2879,14 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:bodyPr rot="5400000" vert="horz"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Time in seconds</a:t>
                 </a:r>
               </a:p>
@@ -2889,7 +2899,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95621056"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="89853888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2898,6 +2918,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -2936,8 +2966,8 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>8176</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>79424</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>122924</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3249,7 +3279,7 @@
   <dimension ref="A1:N340"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M31" sqref="M30:N31"/>
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>